<commit_message>
Editando relatórios para formatar em um só arquivo para PDF
</commit_message>
<xml_diff>
--- a/coleta-manhente.xlsx
+++ b/coleta-manhente.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="-15" windowWidth="19260" windowHeight="4965" activeTab="2"/>
+    <workbookView xWindow="-15" yWindow="-15" windowWidth="19260" windowHeight="4965"/>
   </bookViews>
   <sheets>
     <sheet name="Médias" sheetId="1" r:id="rId1"/>
@@ -230,7 +230,7 @@
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="3"/>
   <c:chart>
     <c:title>
@@ -480,11 +480,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75014912"/>
-        <c:axId val="75017216"/>
+        <c:axId val="75685888"/>
+        <c:axId val="75687808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75014912"/>
+        <c:axId val="75685888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -508,14 +508,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75017216"/>
+        <c:crossAx val="75687808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75017216"/>
+        <c:axId val="75687808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -541,7 +541,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75014912"/>
+        <c:crossAx val="75685888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -554,7 +554,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000047" footer="0.31496062000000047"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000052" footer="0.31496062000000052"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -562,7 +562,7 @@
 
 <file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="4"/>
   <c:chart>
     <c:title>
@@ -800,11 +800,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76715136"/>
-        <c:axId val="76717056"/>
+        <c:axId val="76247424"/>
+        <c:axId val="76249344"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76715136"/>
+        <c:axId val="76247424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -828,14 +828,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76717056"/>
+        <c:crossAx val="76249344"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76717056"/>
+        <c:axId val="76249344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -861,7 +861,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76715136"/>
+        <c:crossAx val="76247424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -874,7 +874,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -882,7 +882,7 @@
 
 <file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="5"/>
   <c:chart>
     <c:title>
@@ -1137,11 +1137,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76838016"/>
-        <c:axId val="76839936"/>
+        <c:axId val="76095872"/>
+        <c:axId val="76097792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76838016"/>
+        <c:axId val="76095872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1165,14 +1165,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76839936"/>
+        <c:crossAx val="76097792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76839936"/>
+        <c:axId val="76097792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1198,7 +1198,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76838016"/>
+        <c:crossAx val="76095872"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1211,7 +1211,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1219,7 +1219,7 @@
 
 <file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="6"/>
   <c:chart>
     <c:title>
@@ -1441,11 +1441,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76895744"/>
-        <c:axId val="76897664"/>
+        <c:axId val="76288768"/>
+        <c:axId val="76290688"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76895744"/>
+        <c:axId val="76288768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1469,14 +1469,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76897664"/>
+        <c:crossAx val="76290688"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76897664"/>
+        <c:axId val="76290688"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1502,7 +1502,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76895744"/>
+        <c:crossAx val="76288768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1515,7 +1515,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1523,7 +1523,7 @@
 
 <file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1714,11 +1714,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76744576"/>
-        <c:axId val="76754944"/>
+        <c:axId val="76330112"/>
+        <c:axId val="76332032"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76744576"/>
+        <c:axId val="76330112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1742,14 +1742,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76754944"/>
+        <c:crossAx val="76332032"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76754944"/>
+        <c:axId val="76332032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1775,7 +1775,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76744576"/>
+        <c:crossAx val="76330112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1788,7 +1788,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1796,7 +1796,7 @@
 
 <file path=xl/charts/chart14.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -1987,11 +1987,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76790016"/>
-        <c:axId val="76796288"/>
+        <c:axId val="76359168"/>
+        <c:axId val="76361088"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76790016"/>
+        <c:axId val="76359168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2015,14 +2015,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76796288"/>
+        <c:crossAx val="76361088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76796288"/>
+        <c:axId val="76361088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2048,7 +2048,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76790016"/>
+        <c:crossAx val="76359168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2061,7 +2061,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2069,7 +2069,7 @@
 
 <file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2260,11 +2260,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77224576"/>
-        <c:axId val="77243136"/>
+        <c:axId val="76412800"/>
+        <c:axId val="76423168"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77224576"/>
+        <c:axId val="76412800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2288,14 +2288,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77243136"/>
+        <c:crossAx val="76423168"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77243136"/>
+        <c:axId val="76423168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2321,7 +2321,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77224576"/>
+        <c:crossAx val="76412800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2334,7 +2334,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000091" footer="0.31496062000000091"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2342,7 +2342,7 @@
 
 <file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -2530,11 +2530,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77278208"/>
-        <c:axId val="77292672"/>
+        <c:axId val="76462336"/>
+        <c:axId val="76476800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77278208"/>
+        <c:axId val="76462336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2558,14 +2558,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77292672"/>
+        <c:crossAx val="76476800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77292672"/>
+        <c:axId val="76476800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2591,7 +2591,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77278208"/>
+        <c:crossAx val="76462336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2604,7 +2604,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000091" footer="0.31496062000000091"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000097" footer="0.31496062000000097"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2612,7 +2612,7 @@
 
 <file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="3"/>
   <c:chart>
     <c:title>
@@ -2862,11 +2862,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77426688"/>
-        <c:axId val="77428608"/>
+        <c:axId val="76536832"/>
+        <c:axId val="76547200"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77426688"/>
+        <c:axId val="76536832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2890,14 +2890,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77428608"/>
+        <c:crossAx val="76547200"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77428608"/>
+        <c:axId val="76547200"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2923,7 +2923,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77426688"/>
+        <c:crossAx val="76536832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2936,7 +2936,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -2944,7 +2944,7 @@
 
 <file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="4"/>
   <c:chart>
     <c:title>
@@ -3182,11 +3182,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77459840"/>
-        <c:axId val="77461760"/>
+        <c:axId val="76582272"/>
+        <c:axId val="76596736"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77459840"/>
+        <c:axId val="76582272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3210,14 +3210,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77461760"/>
+        <c:crossAx val="76596736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77461760"/>
+        <c:axId val="76596736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3243,7 +3243,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77459840"/>
+        <c:crossAx val="76582272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3256,7 +3256,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000091" footer="0.31496062000000091"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3264,7 +3264,7 @@
 
 <file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="5"/>
   <c:chart>
     <c:title>
@@ -3519,11 +3519,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77378304"/>
-        <c:axId val="77380224"/>
+        <c:axId val="76779520"/>
+        <c:axId val="76781440"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77378304"/>
+        <c:axId val="76779520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3547,14 +3547,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77380224"/>
+        <c:crossAx val="76781440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77380224"/>
+        <c:axId val="76781440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3580,7 +3580,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77378304"/>
+        <c:crossAx val="76779520"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3593,7 +3593,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000091" footer="0.31496062000000091"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3601,7 +3601,7 @@
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="4"/>
   <c:chart>
     <c:title>
@@ -3839,11 +3839,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="74683904"/>
-        <c:axId val="74685824"/>
+        <c:axId val="75706752"/>
+        <c:axId val="75708672"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="74683904"/>
+        <c:axId val="75706752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3867,14 +3867,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74685824"/>
+        <c:crossAx val="75708672"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74685824"/>
+        <c:axId val="75708672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3900,7 +3900,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="74683904"/>
+        <c:crossAx val="75706752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3913,7 +3913,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000052" footer="0.31496062000000052"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000058" footer="0.31496062000000058"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -3921,7 +3921,7 @@
 
 <file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="6"/>
   <c:chart>
     <c:title>
@@ -4143,11 +4143,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77747328"/>
-        <c:axId val="77749248"/>
+        <c:axId val="77148544"/>
+        <c:axId val="77150464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77747328"/>
+        <c:axId val="77148544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4171,14 +4171,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77749248"/>
+        <c:crossAx val="77150464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77749248"/>
+        <c:axId val="77150464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4204,7 +4204,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77747328"/>
+        <c:crossAx val="77148544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4217,7 +4217,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000091" footer="0.31496062000000091"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000097" footer="0.31496062000000097"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4225,7 +4225,7 @@
 
 <file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4416,11 +4416,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77870976"/>
-        <c:axId val="77881344"/>
+        <c:axId val="77198464"/>
+        <c:axId val="77200384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77870976"/>
+        <c:axId val="77198464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4444,14 +4444,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77881344"/>
+        <c:crossAx val="77200384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77881344"/>
+        <c:axId val="77200384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4477,7 +4477,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77870976"/>
+        <c:crossAx val="77198464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4490,7 +4490,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000091" footer="0.31496062000000091"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4498,7 +4498,7 @@
 
 <file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4689,11 +4689,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77916416"/>
-        <c:axId val="77803904"/>
+        <c:axId val="76846592"/>
+        <c:axId val="76848512"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77916416"/>
+        <c:axId val="76846592"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4717,14 +4717,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77803904"/>
+        <c:crossAx val="76848512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77803904"/>
+        <c:axId val="76848512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4750,7 +4750,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77916416"/>
+        <c:crossAx val="76846592"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4763,7 +4763,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000091" footer="0.31496062000000091"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000097" footer="0.31496062000000097"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -4771,7 +4771,7 @@
 
 <file path=xl/charts/chart23.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -4962,11 +4962,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77826688"/>
-        <c:axId val="77837056"/>
+        <c:axId val="77227904"/>
+        <c:axId val="77238272"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77826688"/>
+        <c:axId val="77227904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4990,14 +4990,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77837056"/>
+        <c:crossAx val="77238272"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77837056"/>
+        <c:axId val="77238272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5023,7 +5023,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77826688"/>
+        <c:crossAx val="77227904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5036,7 +5036,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000097" footer="0.31496062000000097"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000102" footer="0.31496062000000102"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5044,7 +5044,7 @@
 
 <file path=xl/charts/chart24.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -5232,11 +5232,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="77958144"/>
-        <c:axId val="77964416"/>
+        <c:axId val="77342976"/>
+        <c:axId val="77349248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="77958144"/>
+        <c:axId val="77342976"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5260,14 +5260,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77964416"/>
+        <c:crossAx val="77349248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77964416"/>
+        <c:axId val="77349248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5293,7 +5293,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="77958144"/>
+        <c:crossAx val="77342976"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5306,7 +5306,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000102" footer="0.31496062000000102"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000108" footer="0.31496062000000108"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5314,7 +5314,7 @@
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="5"/>
   <c:chart>
     <c:title>
@@ -5566,11 +5566,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75257728"/>
-        <c:axId val="75276288"/>
+        <c:axId val="75760384"/>
+        <c:axId val="75762304"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75257728"/>
+        <c:axId val="75760384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5594,14 +5594,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75276288"/>
+        <c:crossAx val="75762304"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75276288"/>
+        <c:axId val="75762304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5627,7 +5627,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75257728"/>
+        <c:crossAx val="75760384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5640,7 +5640,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000052" footer="0.31496062000000052"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000058" footer="0.31496062000000058"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5648,7 +5648,7 @@
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="6"/>
   <c:chart>
     <c:title>
@@ -5675,6 +5675,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -5869,11 +5870,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75192576"/>
-        <c:axId val="75198848"/>
+        <c:axId val="75801728"/>
+        <c:axId val="75803648"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75192576"/>
+        <c:axId val="75801728"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5894,16 +5895,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75198848"/>
+        <c:crossAx val="75803648"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75198848"/>
+        <c:axId val="75803648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5925,22 +5927,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75192576"/>
+        <c:crossAx val="75801728"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000058" footer="0.31496062000000058"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -5948,7 +5952,7 @@
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -5966,6 +5970,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -6138,11 +6143,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75377664"/>
-        <c:axId val="75379840"/>
+        <c:axId val="75876224"/>
+        <c:axId val="75882496"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75377664"/>
+        <c:axId val="75876224"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6163,16 +6168,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75379840"/>
+        <c:crossAx val="75882496"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75379840"/>
+        <c:axId val="75882496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6194,22 +6200,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75377664"/>
+        <c:crossAx val="75876224"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000052" footer="0.31496062000000052"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000058" footer="0.31496062000000058"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6217,7 +6225,7 @@
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -6235,6 +6243,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -6407,11 +6416,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75410816"/>
-        <c:axId val="75417088"/>
+        <c:axId val="75909376"/>
+        <c:axId val="75927936"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75410816"/>
+        <c:axId val="75909376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6432,16 +6441,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75417088"/>
+        <c:crossAx val="75927936"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75417088"/>
+        <c:axId val="75927936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6463,22 +6473,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75410816"/>
+        <c:crossAx val="75909376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000058" footer="0.31496062000000058"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6486,7 +6498,7 @@
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -6504,6 +6516,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -6673,11 +6686,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="75333632"/>
-        <c:axId val="75335552"/>
+        <c:axId val="76028544"/>
+        <c:axId val="76043008"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75333632"/>
+        <c:axId val="76028544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6698,16 +6711,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75335552"/>
+        <c:crossAx val="76043008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="75335552"/>
+        <c:axId val="76043008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6729,22 +6743,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="75333632"/>
+        <c:crossAx val="76028544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -6752,7 +6768,7 @@
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:chart>
     <c:title>
       <c:tx>
@@ -6770,6 +6786,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
     </c:title>
     <c:plotArea>
       <c:layout/>
@@ -6939,11 +6956,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76632448"/>
-        <c:axId val="76634368"/>
+        <c:axId val="76073984"/>
+        <c:axId val="75957376"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76632448"/>
+        <c:axId val="76073984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6964,16 +6981,17 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76634368"/>
+        <c:crossAx val="75957376"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76634368"/>
+        <c:axId val="75957376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -6995,22 +7013,24 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76632448"/>
+        <c:crossAx val="76073984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000075" footer="0.31496062000000075"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000086" footer="0.31496062000000086"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -7018,7 +7038,7 @@
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:lang val="pt-BR"/>
+  <c:lang val="en-US"/>
   <c:style val="3"/>
   <c:chart>
     <c:title>
@@ -7268,11 +7288,11 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="76595968"/>
-        <c:axId val="76597888"/>
+        <c:axId val="76169216"/>
+        <c:axId val="76171136"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="76595968"/>
+        <c:axId val="76169216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7296,14 +7316,14 @@
           <c:layout/>
         </c:title>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76597888"/>
+        <c:crossAx val="76171136"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="76597888"/>
+        <c:axId val="76171136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7329,7 +7349,7 @@
         </c:title>
         <c:numFmt formatCode="0.0000" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="76595968"/>
+        <c:crossAx val="76169216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -7342,7 +7362,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000058" footer="0.31496062000000058"/>
+    <c:pageMargins b="0.78740157499999996" l="0.511811024" r="0.511811024" t="0.78740157499999996" header="0.31496062000000064" footer="0.31496062000000064"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -8084,9 +8104,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8124,7 +8144,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -8194,7 +8214,7 @@
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8370,8 +8390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IW29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:C29"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9157,8 +9177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IW29"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:C29"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -9945,8 +9965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:IW29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:C29"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>

</xml_diff>